<commit_message>
Détection de perte de ligne op
</commit_message>
<xml_diff>
--- a/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/speeds.xlsx
+++ b/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/speeds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MountWD\Donnees\ODJ\008_iao_wrk\VoRoboticsAsso\00-AutresProjetsDuLab\0025-permiC_2019\project\_01-docs\_01-userDoc\documentionProjetToWeb\source\advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{551C8AE1-2284-4843-AD0A-82982A5A3490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F14EDC-8E0D-4F26-B689-64D9AB7C4ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" xr2:uid="{D223448C-53F8-4087-A663-606D00999F43}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>VBAT</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Vit km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPM à vide </t>
+  </si>
+  <si>
+    <t>VBAT à VIDE</t>
   </si>
 </sst>
 </file>
@@ -72,8 +78,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -112,8 +118,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65050AF-28D5-45EB-A45C-F6180238850D}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +447,7 @@
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -452,7 +458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -463,7 +469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -482,8 +488,14 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7.45</v>
       </c>
@@ -506,7 +518,7 @@
         <v>1.5428571428571427</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7.42</v>
       </c>
@@ -529,7 +541,7 @@
         <v>1.1489361702127658</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.4</v>
       </c>
@@ -552,7 +564,7 @@
         <v>0.6467065868263473</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>90</v>
       </c>
@@ -572,7 +584,7 @@
         <v>1.2811387900355873</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7.65</v>
       </c>
@@ -593,6 +605,69 @@
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>1.6615384615384616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7.5</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D9" s="1">
+        <f>Distance/C9</f>
+        <v>0.64516129032258063</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D9/(Diam_roue*PI())*1000*60</f>
+        <v>189.56420020870908</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" ref="F9" si="1">D9*3.6</f>
+        <v>2.3225806451612905</v>
+      </c>
+      <c r="G9">
+        <v>216</v>
+      </c>
+      <c r="H9">
+        <v>8.07</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7.53</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>4.51</v>
+      </c>
+      <c r="D10" s="1">
+        <f>Distance/C10</f>
+        <v>0.66518847006651893</v>
+      </c>
+      <c r="E10" s="2">
+        <f>D10/(Diam_roue*PI())*1000*60</f>
+        <v>195.44867649013247</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ref="F10" si="2">D10*3.6</f>
+        <v>2.3946784922394682</v>
+      </c>
+      <c r="G10">
+        <v>217</v>
+      </c>
+      <c r="H10">
+        <v>7.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version avec tentative de détection de tag sur le bord de la piste
</commit_message>
<xml_diff>
--- a/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/speeds.xlsx
+++ b/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/speeds.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MountWD\Donnees\ODJ\008_iao_wrk\VoRoboticsAsso\00-AutresProjetsDuLab\0025-permiC_2019\project\_01-docs\_01-userDoc\documentionProjetToWeb\source\advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F14EDC-8E0D-4F26-B689-64D9AB7C4ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7559764C-B50D-4DC3-8D35-C893807E1E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" xr2:uid="{D223448C-53F8-4087-A663-606D00999F43}"/>
+    <workbookView xWindow="14355" yWindow="1575" windowWidth="13365" windowHeight="11145" xr2:uid="{D223448C-53F8-4087-A663-606D00999F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Diam_roue">Feuil1!$B$2</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>VBAT</t>
   </si>
@@ -71,6 +72,21 @@
   </si>
   <si>
     <t>VBAT à VIDE</t>
+  </si>
+  <si>
+    <t>CONS</t>
+  </si>
+  <si>
+    <t>VBAT0</t>
+  </si>
+  <si>
+    <t>comportement sur la piste</t>
+  </si>
+  <si>
+    <t>sortie</t>
+  </si>
+  <si>
+    <t>ok mais limite</t>
   </si>
 </sst>
 </file>
@@ -136,6 +152,1178 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Vitesse vs Vbat</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CONS70</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil2!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil2!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-04A8-48C6-BDD6-9B44A31DCA3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CONS100</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil2!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil2!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>196</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-04A8-48C6-BDD6-9B44A31DCA3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CONS150</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil2!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil2!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-04A8-48C6-BDD6-9B44A31DCA3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="282935768"/>
+        <c:axId val="282936096"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="282935768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="282936096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="282936096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="282935768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>714376</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33176A6C-D98A-40CA-A7B7-31AC3097DDD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65050AF-28D5-45EB-A45C-F6180238850D}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +1635,7 @@
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -458,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -469,7 +1657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -494,8 +1682,11 @@
       <c r="H3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7.45</v>
       </c>
@@ -506,11 +1697,11 @@
         <v>7</v>
       </c>
       <c r="D4" s="1">
-        <f>Distance/C4</f>
+        <f t="shared" ref="D4:D14" si="0">Distance/C4</f>
         <v>0.42857142857142855</v>
       </c>
       <c r="E4" s="2">
-        <f>D4/(Diam_roue*PI())*1000*60</f>
+        <f t="shared" ref="E4:E14" si="1">D4/(Diam_roue*PI())*1000*60</f>
         <v>125.92479013864245</v>
       </c>
       <c r="F4" s="3">
@@ -518,7 +1709,7 @@
         <v>1.5428571428571427</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7.42</v>
       </c>
@@ -529,19 +1720,19 @@
         <v>9.4</v>
       </c>
       <c r="D5" s="1">
-        <f>Distance/C5</f>
+        <f t="shared" si="0"/>
         <v>0.31914893617021273</v>
       </c>
       <c r="E5" s="2">
-        <f>D5/(Diam_roue*PI())*1000*60</f>
+        <f t="shared" si="1"/>
         <v>93.773779890478423</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F8" si="0">D5*3.6</f>
+        <f t="shared" ref="F5:F8" si="2">D5*3.6</f>
         <v>1.1489361702127658</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.4</v>
       </c>
@@ -552,19 +1743,19 @@
         <v>16.7</v>
       </c>
       <c r="D6" s="1">
-        <f>Distance/C6</f>
+        <f t="shared" si="0"/>
         <v>0.17964071856287425</v>
       </c>
       <c r="E6" s="2">
-        <f>D6/(Diam_roue*PI())*1000*60</f>
+        <f t="shared" si="1"/>
         <v>52.782846165898043</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6467065868263473</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>90</v>
       </c>
@@ -572,19 +1763,19 @@
         <v>8.43</v>
       </c>
       <c r="D7" s="1">
-        <f>Distance/C7</f>
+        <f t="shared" si="0"/>
         <v>0.35587188612099646</v>
       </c>
       <c r="E7" s="2">
-        <f>D7/(Diam_roue*PI())*1000*60</f>
+        <f t="shared" si="1"/>
         <v>104.56388267740182</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2811387900355873</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7.65</v>
       </c>
@@ -595,19 +1786,19 @@
         <v>6.5</v>
       </c>
       <c r="D8" s="1">
-        <f>Distance/C8</f>
+        <f t="shared" si="0"/>
         <v>0.46153846153846156</v>
       </c>
       <c r="E8" s="2">
-        <f>D8/(Diam_roue*PI())*1000*60</f>
+        <f t="shared" si="1"/>
         <v>135.6113124569996</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.6615384615384616</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7.5</v>
       </c>
@@ -618,15 +1809,15 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="D9" s="1">
-        <f>Distance/C9</f>
+        <f t="shared" si="0"/>
         <v>0.64516129032258063</v>
       </c>
       <c r="E9" s="2">
-        <f>D9/(Diam_roue*PI())*1000*60</f>
+        <f t="shared" si="1"/>
         <v>189.56420020870908</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9" si="1">D9*3.6</f>
+        <f t="shared" ref="F9" si="3">D9*3.6</f>
         <v>2.3225806451612905</v>
       </c>
       <c r="G9">
@@ -636,7 +1827,7 @@
         <v>8.07</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7.53</v>
       </c>
@@ -647,15 +1838,15 @@
         <v>4.51</v>
       </c>
       <c r="D10" s="1">
-        <f>Distance/C10</f>
+        <f t="shared" si="0"/>
         <v>0.66518847006651893</v>
       </c>
       <c r="E10" s="2">
-        <f>D10/(Diam_roue*PI())*1000*60</f>
+        <f t="shared" si="1"/>
         <v>195.44867649013247</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ref="F10" si="2">D10*3.6</f>
+        <f t="shared" ref="F10" si="4">D10*3.6</f>
         <v>2.3946784922394682</v>
       </c>
       <c r="G10">
@@ -665,12 +1856,441 @@
         <v>7.87</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7.2</v>
+      </c>
+      <c r="B11">
+        <v>130</v>
+      </c>
+      <c r="C11">
+        <v>6.5</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>135.6113124569996</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" ref="F11" si="5">D11*3.6</f>
+        <v>1.6615384615384616</v>
+      </c>
+      <c r="G11">
+        <v>172</v>
+      </c>
+      <c r="H11">
+        <v>7.52</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7.01</v>
+      </c>
+      <c r="B12">
+        <v>120</v>
+      </c>
+      <c r="C12">
+        <v>7.2</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>122.42687930145794</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" ref="F12" si="6">D12*3.6</f>
+        <v>1.5</v>
+      </c>
+      <c r="G12">
+        <v>165</v>
+      </c>
+      <c r="H12">
+        <v>7.52</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7.01</v>
+      </c>
+      <c r="B13">
+        <v>110</v>
+      </c>
+      <c r="C13">
+        <v>8.06</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.37220843672456572</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>109.36396165887064</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ref="F13" si="7">D13*3.6</f>
+        <v>1.3399503722084367</v>
+      </c>
+      <c r="G13">
+        <v>162</v>
+      </c>
+      <c r="H13">
+        <v>7.49</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>115</v>
+      </c>
+      <c r="C14">
+        <v>7.6</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.39473684210526316</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>115.98335933822334</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ref="F14" si="8">D14*3.6</f>
+        <v>1.4210526315789473</v>
+      </c>
+      <c r="G14">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30E9209-D4F3-450E-ACC4-F7F1DE461FF4}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1">
+        <v>70</v>
+      </c>
+      <c r="H1">
+        <v>100</v>
+      </c>
+      <c r="I1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>8.4</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+      <c r="F2">
+        <v>6.5</v>
+      </c>
+      <c r="G2">
+        <v>85</v>
+      </c>
+      <c r="H2">
+        <v>127</v>
+      </c>
+      <c r="I2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C3">
+        <v>140</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>107</v>
+      </c>
+      <c r="H3">
+        <v>144</v>
+      </c>
+      <c r="I3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>136</v>
+      </c>
+      <c r="F4">
+        <v>7.3</v>
+      </c>
+      <c r="G4">
+        <v>108</v>
+      </c>
+      <c r="H4">
+        <v>153</v>
+      </c>
+      <c r="I4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7.6</v>
+      </c>
+      <c r="C5">
+        <v>124</v>
+      </c>
+      <c r="F5">
+        <v>7.6</v>
+      </c>
+      <c r="G5">
+        <v>124</v>
+      </c>
+      <c r="H5">
+        <v>165</v>
+      </c>
+      <c r="I5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>7.3</v>
+      </c>
+      <c r="C6">
+        <v>108</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>136</v>
+      </c>
+      <c r="H6">
+        <v>175</v>
+      </c>
+      <c r="I6">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>107</v>
+      </c>
+      <c r="F7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G7">
+        <v>140</v>
+      </c>
+      <c r="H7">
+        <v>180</v>
+      </c>
+      <c r="I7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6.5</v>
+      </c>
+      <c r="C8">
+        <v>85</v>
+      </c>
+      <c r="F8">
+        <v>8.4</v>
+      </c>
+      <c r="G8">
+        <v>150</v>
+      </c>
+      <c r="H8">
+        <v>196</v>
+      </c>
+      <c r="I8">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>8.4</v>
+      </c>
+      <c r="C10">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>7.6</v>
+      </c>
+      <c r="C13">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>7.3</v>
+      </c>
+      <c r="C14">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>6.5</v>
+      </c>
+      <c r="C16">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>150</v>
+      </c>
+      <c r="B18">
+        <v>8.4</v>
+      </c>
+      <c r="C18">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C19">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>7.6</v>
+      </c>
+      <c r="C21">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>7.3</v>
+      </c>
+      <c r="C22">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>6.5</v>
+      </c>
+      <c r="C24">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:I8">
+    <sortCondition ref="F2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>